<commit_message>
Data_output. Corrigiendo función plot
</commit_message>
<xml_diff>
--- a/data/final/rs_analysis.xlsx
+++ b/data/final/rs_analysis.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E563"/>
+  <dimension ref="A1:E567"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9977,6 +9977,74 @@
         <v>170.595</v>
       </c>
     </row>
+    <row r="564" spans="1:5">
+      <c r="A564" s="2">
+        <v>45419</v>
+      </c>
+      <c r="B564">
+        <v>100</v>
+      </c>
+      <c r="C564">
+        <v>122.959</v>
+      </c>
+      <c r="D564">
+        <v>149.758</v>
+      </c>
+      <c r="E564">
+        <v>169.983</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5">
+      <c r="A565" s="2">
+        <v>45420</v>
+      </c>
+      <c r="B565">
+        <v>100</v>
+      </c>
+      <c r="C565">
+        <v>121.358</v>
+      </c>
+      <c r="D565">
+        <v>147.665</v>
+      </c>
+      <c r="E565">
+        <v>170.227</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5">
+      <c r="A566" s="2">
+        <v>45421</v>
+      </c>
+      <c r="B566">
+        <v>100</v>
+      </c>
+      <c r="C566">
+        <v>119.644</v>
+      </c>
+      <c r="D566">
+        <v>146.82</v>
+      </c>
+      <c r="E566">
+        <v>170.026</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5">
+      <c r="A567" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B567">
+        <v>100</v>
+      </c>
+      <c r="C567">
+        <v>122.629</v>
+      </c>
+      <c r="D567">
+        <v>146.352</v>
+      </c>
+      <c r="E567">
+        <v>165.764</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9984,7 +10052,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C563"/>
+  <dimension ref="A1:C567"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -16183,6 +16251,50 @@
         <v>0.48</v>
       </c>
     </row>
+    <row r="564" spans="1:3">
+      <c r="A564" s="2">
+        <v>45419</v>
+      </c>
+      <c r="B564">
+        <v>1040</v>
+      </c>
+      <c r="C564">
+        <v>-0.48</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3">
+      <c r="A565" s="2">
+        <v>45420</v>
+      </c>
+      <c r="B565">
+        <v>1040</v>
+      </c>
+      <c r="C565">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3">
+      <c r="A566" s="2">
+        <v>45421</v>
+      </c>
+      <c r="B566">
+        <v>1045</v>
+      </c>
+      <c r="C566">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3">
+      <c r="A567" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B567">
+        <v>1040</v>
+      </c>
+      <c r="C567">
+        <v>-0.48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16190,7 +16302,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C563"/>
+  <dimension ref="A1:C567"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -22389,6 +22501,50 @@
         <v>0.166</v>
       </c>
     </row>
+    <row r="564" spans="1:3">
+      <c r="A564" s="2">
+        <v>45419</v>
+      </c>
+      <c r="B564">
+        <v>870</v>
+      </c>
+      <c r="C564">
+        <v>-3.889</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3">
+      <c r="A565" s="2">
+        <v>45420</v>
+      </c>
+      <c r="B565">
+        <v>858.5</v>
+      </c>
+      <c r="C565">
+        <v>-1.331</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3">
+      <c r="A566" s="2">
+        <v>45421</v>
+      </c>
+      <c r="B566">
+        <v>848</v>
+      </c>
+      <c r="C566">
+        <v>-1.231</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3">
+      <c r="A567" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B567">
+        <v>918.5</v>
+      </c>
+      <c r="C567">
+        <v>7.986</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22396,7 +22552,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C563"/>
+  <dimension ref="A1:C567"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -28595,6 +28751,50 @@
         <v>5.641</v>
       </c>
     </row>
+    <row r="564" spans="1:3">
+      <c r="A564" s="2">
+        <v>45419</v>
+      </c>
+      <c r="B564">
+        <v>3902.5</v>
+      </c>
+      <c r="C564">
+        <v>-4.546</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3">
+      <c r="A565" s="2">
+        <v>45420</v>
+      </c>
+      <c r="B565">
+        <v>3846</v>
+      </c>
+      <c r="C565">
+        <v>-1.458</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3">
+      <c r="A566" s="2">
+        <v>45421</v>
+      </c>
+      <c r="B566">
+        <v>3760</v>
+      </c>
+      <c r="C566">
+        <v>-2.261</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3">
+      <c r="A567" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B567">
+        <v>3738</v>
+      </c>
+      <c r="C567">
+        <v>-0.587</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28602,7 +28802,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C563"/>
+  <dimension ref="A1:C567"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -34801,6 +35001,50 @@
         <v>2.082</v>
       </c>
     </row>
+    <row r="564" spans="1:3">
+      <c r="A564" s="2">
+        <v>45419</v>
+      </c>
+      <c r="B564">
+        <v>26440</v>
+      </c>
+      <c r="C564">
+        <v>-0.787</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3">
+      <c r="A565" s="2">
+        <v>45420</v>
+      </c>
+      <c r="B565">
+        <v>26393.6</v>
+      </c>
+      <c r="C565">
+        <v>-0.176</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3">
+      <c r="A566" s="2">
+        <v>45421</v>
+      </c>
+      <c r="B566">
+        <v>26469.95</v>
+      </c>
+      <c r="C566">
+        <v>0.289</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3">
+      <c r="A567" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B567">
+        <v>24615</v>
+      </c>
+      <c r="C567">
+        <v>-7.265</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>